<commit_message>
Restructuring things, added real time into the project
</commit_message>
<xml_diff>
--- a/Project/classificationAttempts.xlsx
+++ b/Project/classificationAttempts.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Heinrich\Documents\Git\NNFL\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JarvisWalker/Documents/Git/NNFL/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17835" windowHeight="11265"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22620" windowHeight="14260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
   <si>
     <t>55, 45 cycles</t>
   </si>
@@ -40,15 +47,56 @@
   <si>
     <t>70, 46 cycles</t>
   </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>down</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -71,26 +119,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -413,13 +457,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:WE35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="TL6" workbookViewId="0">
+      <selection activeCell="WG39" sqref="WG39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>0.632817856182326</v>
       </c>
@@ -2221,7 +2265,7 @@
         <v>-0.904740805574902</v>
       </c>
     </row>
-    <row r="2" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-0.97835040021789899</v>
       </c>
@@ -4023,7 +4067,7 @@
         <v>-0.70988405501643803</v>
       </c>
     </row>
-    <row r="3" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-0.61392192603500795</v>
       </c>
@@ -5825,7 +5869,7 @@
         <v>-0.897152518663619</v>
       </c>
     </row>
-    <row r="4" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-0.53904198904132705</v>
       </c>
@@ -7627,7 +7671,7 @@
         <v>0.65920918295916497</v>
       </c>
     </row>
-    <row r="6" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.632817856182326</v>
       </c>
@@ -9429,7 +9473,7 @@
         <v>-0.904740805574902</v>
       </c>
     </row>
-    <row r="7" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-0.97835040021789899</v>
       </c>
@@ -11231,7 +11275,7 @@
         <v>-0.70988405501643803</v>
       </c>
     </row>
-    <row r="8" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>-0.61392192603500795</v>
       </c>
@@ -13033,7 +13077,7 @@
         <v>-0.897152518663619</v>
       </c>
     </row>
-    <row r="9" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-0.53904198904132705</v>
       </c>
@@ -14835,7 +14879,7 @@
         <v>0.65920918295916497</v>
       </c>
     </row>
-    <row r="11" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.67468779961890601</v>
       </c>
@@ -16635,6 +16679,9 @@
       </c>
       <c r="WB11">
         <v>-0.94170064582351298</v>
+      </c>
+      <c r="WC11" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="WD11">
         <f t="shared" ref="WD11:WD13" si="0">COUNTIF(A11:WB11, "&gt;0")</f>
@@ -16644,7 +16691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>-0.98991734063068804</v>
       </c>
@@ -18444,13 +18491,16 @@
       </c>
       <c r="WB12">
         <v>-0.68707667097546998</v>
+      </c>
+      <c r="WC12" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="WD12">
         <f t="shared" si="0"/>
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>-0.85972582248894203</v>
       </c>
@@ -20250,13 +20300,16 @@
       </c>
       <c r="WB13">
         <v>-0.96835692371280302</v>
+      </c>
+      <c r="WC13" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="WD13">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>-9.2727531946534505E-2</v>
       </c>
@@ -22056,19 +22109,25 @@
       </c>
       <c r="WB14">
         <v>0.23312001269167101</v>
+      </c>
+      <c r="WC14" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="WD14">
         <f>COUNTIF(A14:WB14, "&gt;0")</f>
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:603" x14ac:dyDescent="0.2">
+      <c r="WC15" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="WD15">
         <f>SUM(WD11:WD14)</f>
         <v>397</v>
       </c>
     </row>
-    <row r="16" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.632817856182326</v>
       </c>
@@ -23869,15 +23928,18 @@
       <c r="WB16">
         <v>-0.904740805574902</v>
       </c>
+      <c r="WC16" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="WD16">
-        <f t="shared" ref="WD15:WD34" si="1">COUNTIF(A16:WB16, "&gt;0")</f>
+        <f t="shared" ref="WD16:WD34" si="1">COUNTIF(A16:WB16, "&gt;0")</f>
         <v>83</v>
       </c>
       <c r="WE16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>-0.97835040021789899</v>
       </c>
@@ -25677,13 +25739,16 @@
       </c>
       <c r="WB17">
         <v>-0.70988405501643803</v>
+      </c>
+      <c r="WC17" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="WD17">
         <f t="shared" si="1"/>
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>-0.61392192603500795</v>
       </c>
@@ -27483,13 +27548,16 @@
       </c>
       <c r="WB18">
         <v>-0.897152518663619</v>
+      </c>
+      <c r="WC18" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="WD18">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>-0.53904198904132705</v>
       </c>
@@ -29289,22 +29357,28 @@
       </c>
       <c r="WB19">
         <v>0.65920918295916497</v>
+      </c>
+      <c r="WC19" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="WD19">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>0</v>
+      </c>
+      <c r="WC20" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="WD20">
         <f>SUM(WD16:WD19)</f>
         <v>413</v>
       </c>
     </row>
-    <row r="21" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>-5.64988472646233E-2</v>
       </c>
@@ -31104,6 +31178,9 @@
       </c>
       <c r="WB21">
         <v>-0.72011807761614499</v>
+      </c>
+      <c r="WC21" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="WD21">
         <f t="shared" si="1"/>
@@ -31113,7 +31190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>-0.665354739149709</v>
       </c>
@@ -32913,13 +32990,16 @@
       </c>
       <c r="WB22">
         <v>-0.52566740032128501</v>
+      </c>
+      <c r="WC22" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="WD22">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>-0.628369439027196</v>
       </c>
@@ -34719,13 +34799,16 @@
       </c>
       <c r="WB23">
         <v>-0.91948684450867402</v>
+      </c>
+      <c r="WC23" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="WD23">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>-0.39284053051659001</v>
       </c>
@@ -36525,19 +36608,25 @@
       </c>
       <c r="WB24">
         <v>-0.24972140037625101</v>
+      </c>
+      <c r="WC24" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="WD24">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:603" x14ac:dyDescent="0.2">
+      <c r="WC25" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="WD25">
         <f>SUM(WD21:WD24)</f>
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>0.75858846862631402</v>
       </c>
@@ -38337,6 +38426,9 @@
       </c>
       <c r="WB26">
         <v>-0.88828435768557801</v>
+      </c>
+      <c r="WC26" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="WD26">
         <f t="shared" si="1"/>
@@ -38346,7 +38438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>-0.95708919778861601</v>
       </c>
@@ -40146,13 +40238,16 @@
       </c>
       <c r="WB27">
         <v>-0.73255206597784694</v>
+      </c>
+      <c r="WC27" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="WD27">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>-0.79486077149689505</v>
       </c>
@@ -41952,13 +42047,16 @@
       </c>
       <c r="WB28">
         <v>-0.97019958249767502</v>
+      </c>
+      <c r="WC28" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="WD28">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>-0.206000322128571</v>
       </c>
@@ -43758,19 +43856,25 @@
       </c>
       <c r="WB29">
         <v>-1.7931026106282801E-2</v>
+      </c>
+      <c r="WC29" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="WD29">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:603" x14ac:dyDescent="0.2">
+      <c r="WC30" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="WD30">
         <f>SUM(WD26:WD29)</f>
         <v>294</v>
       </c>
     </row>
-    <row r="31" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.77743235284433598</v>
       </c>
@@ -45570,6 +45674,9 @@
       </c>
       <c r="WB31">
         <v>-0.86272235268895103</v>
+      </c>
+      <c r="WC31" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="WD31">
         <f t="shared" si="1"/>
@@ -45579,7 +45686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:603" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:603" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>-0.54953294238838102</v>
       </c>
@@ -47379,13 +47486,16 @@
       </c>
       <c r="WB32">
         <v>-0.37837535014183399</v>
+      </c>
+      <c r="WC32" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="WD32">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:602" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>-0.67757770005990703</v>
       </c>
@@ -49185,13 +49295,16 @@
       </c>
       <c r="WB33">
         <v>-0.91012260167744496</v>
+      </c>
+      <c r="WC33" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="WD33">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:602" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>-0.65733505717462704</v>
       </c>
@@ -50991,13 +51104,19 @@
       </c>
       <c r="WB34">
         <v>0.57696645696978699</v>
+      </c>
+      <c r="WC34" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="WD34">
         <f t="shared" si="1"/>
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:602" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:602" x14ac:dyDescent="0.2">
+      <c r="WC35" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="WD35">
         <f>SUM(WD31:WD34)</f>
         <v>394</v>
@@ -51005,10 +51124,885 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:WB1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BS4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A1" s="2">
+        <v>0.40396127147461303</v>
+      </c>
+      <c r="B1" s="2">
+        <v>0.30603233307684602</v>
+      </c>
+      <c r="C1" s="2">
+        <v>0.38758849545465701</v>
+      </c>
+      <c r="D1" s="2">
+        <v>0.429925809719364</v>
+      </c>
+      <c r="E1" s="2">
+        <v>0.26555653162091503</v>
+      </c>
+      <c r="F1" s="2">
+        <v>0.69165712432666504</v>
+      </c>
+      <c r="G1" s="2">
+        <v>0.45094609906286698</v>
+      </c>
+      <c r="H1" s="2">
+        <v>0.18255297094840001</v>
+      </c>
+      <c r="I1" s="2">
+        <v>0.92463088935847604</v>
+      </c>
+      <c r="J1" s="2">
+        <v>0.73339772861752806</v>
+      </c>
+      <c r="K1" s="2">
+        <v>0.73515353019058405</v>
+      </c>
+      <c r="L1" s="2">
+        <v>4.8993274535606902E-2</v>
+      </c>
+      <c r="M1" s="2">
+        <v>0.87138073528885895</v>
+      </c>
+      <c r="N1" s="2">
+        <v>0.61926600602804405</v>
+      </c>
+      <c r="O1" s="2">
+        <v>0.70421041431735598</v>
+      </c>
+      <c r="P1" s="2">
+        <v>0.95959635778892804</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>0.68150278651671303</v>
+      </c>
+      <c r="R1" s="2">
+        <v>0.29536934937940901</v>
+      </c>
+      <c r="S1" s="2">
+        <v>0.38269143058731703</v>
+      </c>
+      <c r="T1" s="2">
+        <v>0.777536222641943</v>
+      </c>
+      <c r="U1" s="2">
+        <v>0.59046943179330103</v>
+      </c>
+      <c r="V1" s="2">
+        <v>0.348124105748641</v>
+      </c>
+      <c r="W1" s="2">
+        <v>0.39530663576922898</v>
+      </c>
+      <c r="X1" s="2">
+        <v>8.3932634307396795E-2</v>
+      </c>
+      <c r="Y1" s="2">
+        <v>0.85707331999201097</v>
+      </c>
+      <c r="Z1" s="2">
+        <v>0.59169518036843305</v>
+      </c>
+      <c r="AA1" s="2">
+        <v>0.56321839279751296</v>
+      </c>
+      <c r="AB1" s="2">
+        <v>0.63367480176052104</v>
+      </c>
+      <c r="AC1" s="2">
+        <v>0.211572100595186</v>
+      </c>
+      <c r="AD1" s="2">
+        <v>0.139935200410778</v>
+      </c>
+      <c r="AE1" s="2">
+        <v>0.131225747226798</v>
+      </c>
+      <c r="AF1" s="2">
+        <v>7.9225768237503894E-2</v>
+      </c>
+      <c r="AG1" s="2">
+        <v>4.9894768574659402E-2</v>
+      </c>
+      <c r="AH1" s="2">
+        <v>0.93508583568373405</v>
+      </c>
+      <c r="AI1" s="2">
+        <v>0.46269095055388898</v>
+      </c>
+      <c r="AJ1" s="2">
+        <v>0.83536006044155098</v>
+      </c>
+      <c r="AK1" s="2">
+        <v>0.78632760291634296</v>
+      </c>
+      <c r="AL1" s="2">
+        <v>0.18901040176707901</v>
+      </c>
+      <c r="AM1" s="2">
+        <v>0.149011501353949</v>
+      </c>
+      <c r="AN1" s="2">
+        <v>0.28851311414375902</v>
+      </c>
+      <c r="AO1" s="2">
+        <v>0.80054479934905798</v>
+      </c>
+      <c r="AP1" s="2">
+        <v>6.8775698186297501E-2</v>
+      </c>
+      <c r="AQ1" s="2">
+        <v>0.75416710309496404</v>
+      </c>
+      <c r="AR1" s="2">
+        <v>0.912916431866716</v>
+      </c>
+      <c r="AS1" s="2">
+        <v>0.929373494541887</v>
+      </c>
+      <c r="AT1" s="2">
+        <v>0.22504778253124999</v>
+      </c>
+      <c r="AU1" s="2">
+        <v>0.98690959455957095</v>
+      </c>
+      <c r="AV1" s="2">
+        <v>0.29478084605682098</v>
+      </c>
+      <c r="AW1" s="2">
+        <v>0.68664108442461602</v>
+      </c>
+      <c r="AX1" s="2">
+        <v>0.14660902930865299</v>
+      </c>
+      <c r="AY1" s="2">
+        <v>0.291839978575402</v>
+      </c>
+      <c r="AZ1" s="2">
+        <v>1.35114943336248E-2</v>
+      </c>
+      <c r="BA1" s="2">
+        <v>0.165147453757541</v>
+      </c>
+      <c r="BB1" s="2">
+        <v>3.5466453735454498E-2</v>
+      </c>
+      <c r="BC1" s="2">
+        <v>0.81204680182753797</v>
+      </c>
+      <c r="BD1" s="2">
+        <v>0.38515596897010201</v>
+      </c>
+      <c r="BE1" s="2">
+        <v>5.6540722714000798E-2</v>
+      </c>
+      <c r="BF1" s="2">
+        <v>0.98357749056243704</v>
+      </c>
+      <c r="BG1" s="2">
+        <v>0.69671325127982398</v>
+      </c>
+      <c r="BH1" s="2">
+        <v>0.16393306427152299</v>
+      </c>
+      <c r="BI1" s="2">
+        <v>0.72128492898346797</v>
+      </c>
+      <c r="BJ1" s="2">
+        <v>0.87275159036794103</v>
+      </c>
+      <c r="BK1" s="2">
+        <v>0.48082041528886599</v>
+      </c>
+      <c r="BL1" s="2">
+        <v>0.75452767628281003</v>
+      </c>
+      <c r="BM1" s="2">
+        <v>8.4804972084489699E-2</v>
+      </c>
+      <c r="BN1" s="2">
+        <v>0.65255555135271104</v>
+      </c>
+      <c r="BO1" s="2">
+        <v>0.17727149901009401</v>
+      </c>
+      <c r="BP1" s="2">
+        <v>0.202215422798358</v>
+      </c>
+      <c r="BQ1" s="2">
+        <v>0.78851386258654699</v>
+      </c>
+      <c r="BR1" s="2">
+        <v>0.62532301444832705</v>
+      </c>
+      <c r="BS1" s="2">
+        <v>0.20757569619313701</v>
+      </c>
+    </row>
+    <row r="2" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0.72487345992437902</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.36975818984429698</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.91552237178279805</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.43424650288907302</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.78334978314917203</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.92101210999849403</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.65380852327780603</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.52600404576815196</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.129663593047772</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.69669031305106099</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.26846997373235298</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0.19242397246753801</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0.77787983770766</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0.48525627456125198</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0.747734276166925</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0.69747622614039995</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>0.28709038287043198</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0.51610410769637804</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0.59691581265494298</v>
+      </c>
+      <c r="T2" s="2">
+        <v>0.235261727538983</v>
+      </c>
+      <c r="U2" s="2">
+        <v>8.4535049482551194E-2</v>
+      </c>
+      <c r="V2" s="2">
+        <v>0.86251892746300396</v>
+      </c>
+      <c r="W2" s="2">
+        <v>0.75307829719295405</v>
+      </c>
+      <c r="X2" s="2">
+        <v>0.22839073954508701</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>0.34814526117440903</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>5.3436722895975002E-2</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>0.64441309908228395</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>0.40388074867614698</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>1.2916750139973799E-2</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>0.79015943517365195</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>0.72225470534330205</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>0.37031160411133202</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>0.46778831290294698</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>0.206415946152502</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>0.10473641254676801</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>0.36510452486641798</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>2.0477366618503998E-2</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>0.64347541788770302</v>
+      </c>
+      <c r="AM2" s="2">
+        <v>0.43453168235085998</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>0.95028297738954404</v>
+      </c>
+      <c r="AO2" s="2">
+        <v>0.983686736041534</v>
+      </c>
+      <c r="AP2" s="2">
+        <v>0.60066048645911096</v>
+      </c>
+      <c r="AQ2" s="2">
+        <v>0.344119986760482</v>
+      </c>
+      <c r="AR2" s="2">
+        <v>0.44232020577807601</v>
+      </c>
+      <c r="AS2" s="2">
+        <v>0.77931154462915397</v>
+      </c>
+      <c r="AT2" s="2">
+        <v>5.1552809273561102E-2</v>
+      </c>
+      <c r="AU2" s="2">
+        <v>0.88043823245563002</v>
+      </c>
+      <c r="AV2" s="2">
+        <v>0.32626085235456798</v>
+      </c>
+      <c r="AW2" s="2">
+        <v>7.4253161107731697E-2</v>
+      </c>
+      <c r="AX2" s="2">
+        <v>0.89622341563179098</v>
+      </c>
+      <c r="AY2" s="2">
+        <v>0.81195443073981</v>
+      </c>
+      <c r="AZ2" s="2">
+        <v>0.11804479096823101</v>
+      </c>
+      <c r="BA2" s="2">
+        <v>0.83309275366442304</v>
+      </c>
+      <c r="BB2" s="2">
+        <v>0.25296406844741898</v>
+      </c>
+      <c r="BC2" s="2">
+        <v>0.273002832875051</v>
+      </c>
+      <c r="BD2" s="2">
+        <v>3.6391857812876002E-2</v>
+      </c>
+      <c r="BE2" s="2">
+        <v>0.41558216489474697</v>
+      </c>
+      <c r="BF2" s="2">
+        <v>0.71122903483191302</v>
+      </c>
+      <c r="BG2" s="2">
+        <v>5.9114913645378797E-2</v>
+      </c>
+      <c r="BH2" s="2">
+        <v>3.7501840522280498E-4</v>
+      </c>
+      <c r="BI2" s="2">
+        <v>0.33297956298882803</v>
+      </c>
+      <c r="BJ2" s="2">
+        <v>0.39717523388170001</v>
+      </c>
+      <c r="BK2" s="2">
+        <v>0.61874863675240999</v>
+      </c>
+      <c r="BL2" s="2">
+        <v>0.76644406180727298</v>
+      </c>
+      <c r="BM2" s="2">
+        <v>0.204515455703459</v>
+      </c>
+      <c r="BN2" s="2">
+        <v>0.45862138245349399</v>
+      </c>
+      <c r="BO2" s="2">
+        <v>0.16810021661725499</v>
+      </c>
+      <c r="BP2" s="2">
+        <v>0.22377665995218299</v>
+      </c>
+      <c r="BQ2" s="2">
+        <v>0.394017799177658</v>
+      </c>
+      <c r="BR2" s="2">
+        <v>0.60999918378832796</v>
+      </c>
+      <c r="BS2" s="2">
+        <v>0.78520622701672504</v>
+      </c>
+    </row>
+    <row r="3" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>0.97125301660846197</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.83715928728199596</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.21162212171325201</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.26625810614665701</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.31998650739940199</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.25545373347079797</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.49498500481282298</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.60638162653350103</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.71146564320580197</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.31756580861694</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.47737933269412097</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4.9209263782414601E-2</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.174677489830218</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0.86971533472797602</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0.86701716630489201</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0.27462371371618799</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0.24494480231206001</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0.88962297843456895</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0.83888305895317905</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0.89719550016640404</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0.551560660575378</v>
+      </c>
+      <c r="V3" s="2">
+        <v>0.10877269338690899</v>
+      </c>
+      <c r="W3" s="2">
+        <v>0.41544113948590999</v>
+      </c>
+      <c r="X3" s="2">
+        <v>0.53656598547511503</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>0.36763085986383898</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>0.466451512075853</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>0.23744502887952201</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>0.39476764593534802</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>0.88641796171085296</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>0.56036036849781301</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>0.855257430744364</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>0.60457543364701205</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>0.889830271505612</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>0.61354178774398804</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>0.39866587247578</v>
+      </c>
+      <c r="AJ3" s="2">
+        <v>0.48212423437996299</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>0.22731747939982999</v>
+      </c>
+      <c r="AL3" s="2">
+        <v>0.99933984761556705</v>
+      </c>
+      <c r="AM3" s="2">
+        <v>0.40336815839010698</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>0.44177891316970302</v>
+      </c>
+      <c r="AO3" s="2">
+        <v>0.21317670403628999</v>
+      </c>
+      <c r="AP3" s="2">
+        <v>0.83524893406440404</v>
+      </c>
+      <c r="AQ3" s="2">
+        <v>0.95744295920710498</v>
+      </c>
+      <c r="AR3" s="2">
+        <v>0.485981280603479</v>
+      </c>
+      <c r="AS3" s="2">
+        <v>0.92129289592399899</v>
+      </c>
+      <c r="AT3" s="2">
+        <v>0.190321758260316</v>
+      </c>
+      <c r="AU3" s="2">
+        <v>0.359063243779356</v>
+      </c>
+      <c r="AV3" s="2">
+        <v>4.6536003114506803E-3</v>
+      </c>
+      <c r="AW3" s="2">
+        <v>0.694865347774002</v>
+      </c>
+      <c r="AX3" s="2">
+        <v>0.52677638420991602</v>
+      </c>
+      <c r="AY3" s="2">
+        <v>1.16419035481269E-2</v>
+      </c>
+      <c r="AZ3" s="2">
+        <v>0.530060959620826</v>
+      </c>
+      <c r="BA3" s="2">
+        <v>0.19910518830751001</v>
+      </c>
+      <c r="BB3" s="2">
+        <v>0.83305099807678895</v>
+      </c>
+      <c r="BC3" s="2">
+        <v>0.82765209062688705</v>
+      </c>
+      <c r="BD3" s="2">
+        <v>0.91626609464458098</v>
+      </c>
+      <c r="BE3" s="2">
+        <v>0.70105796288785405</v>
+      </c>
+      <c r="BF3" s="2">
+        <v>0.194402479915044</v>
+      </c>
+      <c r="BG3" s="2">
+        <v>0.37388002572855999</v>
+      </c>
+      <c r="BH3" s="2">
+        <v>0.926523240602943</v>
+      </c>
+      <c r="BI3" s="2">
+        <v>0.31141605222736501</v>
+      </c>
+      <c r="BJ3" s="2">
+        <v>0.165433178696509</v>
+      </c>
+      <c r="BK3" s="2">
+        <v>1.7853863532553301E-2</v>
+      </c>
+      <c r="BL3" s="2">
+        <v>0.87429454329197898</v>
+      </c>
+      <c r="BM3" s="2">
+        <v>0.65776349419845503</v>
+      </c>
+      <c r="BN3" s="2">
+        <v>4.8292350453640602E-2</v>
+      </c>
+      <c r="BO3" s="2">
+        <v>4.3412856378376198E-2</v>
+      </c>
+      <c r="BP3" s="2">
+        <v>0.73365841256215403</v>
+      </c>
+      <c r="BQ3" s="2">
+        <v>0.86497539012357305</v>
+      </c>
+      <c r="BR3" s="2">
+        <v>0.91988310331805101</v>
+      </c>
+      <c r="BS3" s="2">
+        <v>0.60858449375749002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>0.109083263348554</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.26561342039232999</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.161212312745833</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.56169998511748898</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.50737420057898197</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.29218800063628297</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.122431152935718</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.70647081505520903</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.72677882262118199</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.28293537825697501</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.14606723681683401</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.74891540972996995</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.77970570177865295</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.90558567615562602</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0.62560804274270598</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.454917789834824</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>9.5055731221874495E-2</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0.71893627126550996</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0.89628225479874701</v>
+      </c>
+      <c r="T4" s="2">
+        <v>6.8011900357593399E-2</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0.80053231600979402</v>
+      </c>
+      <c r="V4" s="2">
+        <v>8.4559565402248196E-2</v>
+      </c>
+      <c r="W4" s="2">
+        <v>0.99094728613617999</v>
+      </c>
+      <c r="X4" s="2">
+        <v>0.15969170063494201</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>0.42837486261532298</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>0.107814660563944</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>0.40259318465681798</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>0.88590629327513604</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>0.73844910316008705</v>
+      </c>
+      <c r="AD4" s="2">
+        <v>0.35192822899818599</v>
+      </c>
+      <c r="AE4" s="2">
+        <v>8.4199683512323306E-2</v>
+      </c>
+      <c r="AF4" s="2">
+        <v>0.52423804420573294</v>
+      </c>
+      <c r="AG4" s="2">
+        <v>0.29911935774758502</v>
+      </c>
+      <c r="AH4" s="2">
+        <v>0.76533453913677296</v>
+      </c>
+      <c r="AI4" s="2">
+        <v>0.87097142413476603</v>
+      </c>
+      <c r="AJ4" s="2">
+        <v>0.226262498747893</v>
+      </c>
+      <c r="AK4" s="2">
+        <v>0.29815460323180898</v>
+      </c>
+      <c r="AL4" s="2">
+        <v>0.30677752273833397</v>
+      </c>
+      <c r="AM4" s="2">
+        <v>0.97935832731170502</v>
+      </c>
+      <c r="AN4" s="2">
+        <v>6.8570030253954597E-2</v>
+      </c>
+      <c r="AO4" s="2">
+        <v>0.74391040548449805</v>
+      </c>
+      <c r="AP4" s="2">
+        <v>0.32252316665837599</v>
+      </c>
+      <c r="AQ4" s="2">
+        <v>0.76034298331710903</v>
+      </c>
+      <c r="AR4" s="2">
+        <v>0.94588613872135596</v>
+      </c>
+      <c r="AS4" s="2">
+        <v>6.3441085625432103E-2</v>
+      </c>
+      <c r="AT4" s="2">
+        <v>9.9923959441642299E-2</v>
+      </c>
+      <c r="AU4" s="2">
+        <v>0.57072749688646396</v>
+      </c>
+      <c r="AV4" s="2">
+        <v>7.0369395307986596E-2</v>
+      </c>
+      <c r="AW4" s="2">
+        <v>0.92370114710130002</v>
+      </c>
+      <c r="AX4" s="2">
+        <v>0.45706745562988899</v>
+      </c>
+      <c r="AY4" s="2">
+        <v>0.94324416238003606</v>
+      </c>
+      <c r="AZ4" s="2">
+        <v>0.23677698700925101</v>
+      </c>
+      <c r="BA4" s="2">
+        <v>0.32799117480380502</v>
+      </c>
+      <c r="BB4" s="2">
+        <v>0.25696855819325098</v>
+      </c>
+      <c r="BC4" s="2">
+        <v>0.78501654610604799</v>
+      </c>
+      <c r="BD4" s="2">
+        <v>0.50345328081444396</v>
+      </c>
+      <c r="BE4" s="2">
+        <v>0.27224135653056097</v>
+      </c>
+      <c r="BF4" s="2">
+        <v>0.82803573085131699</v>
+      </c>
+      <c r="BG4" s="2">
+        <v>0.21002910710087699</v>
+      </c>
+      <c r="BH4" s="2">
+        <v>7.4810067024821403E-2</v>
+      </c>
+      <c r="BI4" s="2">
+        <v>2.3703139175094E-2</v>
+      </c>
+      <c r="BJ4" s="2">
+        <v>4.6076859770153397E-2</v>
+      </c>
+      <c r="BK4" s="2">
+        <v>0.219911284183339</v>
+      </c>
+      <c r="BL4" s="2">
+        <v>0.92825041452442103</v>
+      </c>
+      <c r="BM4" s="2">
+        <v>6.4341780335994095E-2</v>
+      </c>
+      <c r="BN4" s="2">
+        <v>0.86827026355880699</v>
+      </c>
+      <c r="BO4" s="2">
+        <v>0.83881369860376598</v>
+      </c>
+      <c r="BP4" s="2">
+        <v>0.65851112730867301</v>
+      </c>
+      <c r="BQ4" s="2">
+        <v>0.34276898966990499</v>
+      </c>
+      <c r="BR4" s="2">
+        <v>0.72446813966823898</v>
+      </c>
+      <c r="BS4" s="2">
+        <v>0.884212185167356</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>